<commit_message>
depot de lab 1 et 2
</commit_message>
<xml_diff>
--- a/Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
+++ b/Excel_Exercice01_MiseEnFormeEtGraphique.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noann\Documents\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55B34E3-0441-4FA8-B42B-3AFBE3564AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3DC963-2662-4E11-9249-914FFF6DB0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultat attendu" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>Total</t>
   </si>
@@ -130,6 +130,9 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Dépense et ventes de 2009</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +146,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;;#,##0.00"/>
     <numFmt numFmtId="169" formatCode="##,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;;#,##0.00"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +297,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color theme="2"/>
@@ -329,8 +326,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial Nova Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +438,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -856,17 +876,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1312,6 +1321,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1320,7 +1340,7 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1534,44 +1554,155 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="36" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="37" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="14" fillId="12" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="43" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="56" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="56" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="58" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="16" borderId="63" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="56" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="13" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="67" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="12" borderId="68" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="16" borderId="69" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="16" borderId="70" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1581,13 +1712,43 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="55" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1597,144 +1758,6 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="43" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="43" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="57" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="58" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="59" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="62" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="16" borderId="64" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="56" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="13" borderId="65" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="66" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="67" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="68" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="69" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="16" borderId="70" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="16" borderId="71" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3674,7 +3697,23 @@
                   <a:srgbClr val="C00000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Dépense 2009</a:t>
+              <a:t>Dépenses</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>2009</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6303,15 +6342,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>201706</xdr:colOff>
+      <xdr:colOff>219849</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>28202</xdr:rowOff>
+      <xdr:rowOff>100773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>284256</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:colOff>302399</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>73692</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6731,44 +6770,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="2" customWidth="1"/>
-    <col min="2" max="7" width="11.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.5703125" style="2" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="9.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="2"/>
-    <col min="18" max="18" width="1.5703125" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="1.54296875" style="2" customWidth="1"/>
+    <col min="2" max="7" width="11.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.54296875" style="2" customWidth="1"/>
+    <col min="9" max="15" width="9.1796875" style="2"/>
+    <col min="16" max="16" width="9.1796875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="2"/>
+    <col min="18" max="18" width="1.54296875" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="69" t="s">
+    <row r="2" spans="2:17" ht="20" x14ac:dyDescent="0.4">
+      <c r="B2" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
     </row>
-    <row r="3" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="3.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -6777,26 +6816,26 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="107"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="107"/>
+      <c r="Q4" s="107"/>
     </row>
-    <row r="5" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="3.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6804,7 +6843,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6820,7 +6859,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="2:17" s="4" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" s="4" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="46" t="s">
         <v>7</v>
       </c>
@@ -6840,7 +6879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
@@ -6861,7 +6900,7 @@
         <v>18105.46</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
@@ -6882,7 +6921,7 @@
         <v>27164.67</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>10</v>
       </c>
@@ -6903,7 +6942,7 @@
         <v>40624.120000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>11</v>
       </c>
@@ -6924,7 +6963,7 @@
         <v>8951.24</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
@@ -6945,7 +6984,7 @@
         <v>8962.11</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -6970,7 +7009,7 @@
         <v>103807.6</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -6986,7 +7025,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="45" t="s">
         <v>2</v>
       </c>
@@ -7006,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>14</v>
       </c>
@@ -7027,7 +7066,7 @@
         <v>50600.09</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="10.5" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
@@ -7048,7 +7087,7 @@
         <v>28167.059999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
         <v>16</v>
       </c>
@@ -7069,7 +7108,7 @@
         <v>24795.49</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
         <v>0</v>
       </c>
@@ -7094,7 +7133,7 @@
         <v>103562.64</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -7110,7 +7149,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="47" t="s">
         <v>1</v>
       </c>
@@ -7130,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="11" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
         <v>0</v>
       </c>
@@ -7175,414 +7214,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" customWidth="1"/>
+    <col min="3" max="6" width="11.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.1796875" style="1" customWidth="1"/>
+    <col min="9" max="15" width="9.1796875" style="1"/>
+    <col min="16" max="16" width="9.1796875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="57" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="59" t="s">
+    <row r="1" spans="1:19" s="56" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="109"/>
     </row>
-    <row r="2" spans="1:17" s="57" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
+    <row r="2" spans="1:19" s="56" customFormat="1" ht="10.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="111"/>
     </row>
-    <row r="3" spans="1:17" s="71" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>13</v>
-      </c>
+    <row r="3" spans="1:19" s="105" customFormat="1" ht="10.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="118" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="119"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
+      <c r="J3" s="119"/>
+      <c r="K3" s="119"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="119"/>
     </row>
-    <row r="4" spans="1:17" s="73" customFormat="1" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
+    <row r="4" spans="1:19" s="105" customFormat="1" ht="10.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="120"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
     </row>
-    <row r="5" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:17" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="110" t="s">
+    <row r="5" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:19" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="76"/>
+      <c r="F7" s="65"/>
     </row>
-    <row r="8" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="111"/>
-      <c r="C8" s="112" t="s">
+    <row r="8" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="113"/>
+      <c r="C8" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="112" t="s">
+      <c r="D8" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="112" t="s">
+      <c r="E8" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="113" t="s">
+      <c r="F8" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="57" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="90" t="s">
+    <row r="9" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="94">
+      <c r="C9" s="83">
         <v>1988.5</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="83">
         <v>2897.35</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="83">
         <v>5223.25</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="66">
         <v>7996.36</v>
       </c>
-      <c r="G9" s="67">
+      <c r="G9" s="63">
         <v>18105.46</v>
       </c>
       <c r="J9" s="55"/>
     </row>
-    <row r="10" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="91" t="s">
+    <row r="10" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="95">
+      <c r="C10" s="84">
         <v>5215</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="84">
         <v>8309.0499999999993</v>
       </c>
-      <c r="E10" s="95">
+      <c r="E10" s="84">
         <v>4287.9799999999996</v>
       </c>
-      <c r="F10" s="78">
+      <c r="F10" s="67">
         <v>9352.64</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="64">
         <v>27164.67</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="90" t="s">
+    <row r="11" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="94">
+      <c r="C11" s="83">
         <v>7832.97</v>
       </c>
-      <c r="D11" s="94">
+      <c r="D11" s="83">
         <v>11299.87</v>
       </c>
-      <c r="E11" s="94">
+      <c r="E11" s="83">
         <v>8264.81</v>
       </c>
-      <c r="F11" s="77">
+      <c r="F11" s="66">
         <v>13226.47</v>
       </c>
-      <c r="G11" s="67">
+      <c r="G11" s="63">
         <v>40624.120000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="91" t="s">
+    <row r="12" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="95">
+      <c r="C12" s="84">
         <v>2337.81</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="84">
         <v>2137.81</v>
       </c>
-      <c r="E12" s="95">
+      <c r="E12" s="84">
         <v>1237.81</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="67">
         <v>3237.81</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="64">
         <v>8951.24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="92" t="s">
+    <row r="13" spans="1:19" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="96">
+      <c r="C13" s="85">
         <v>4336.37</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="85">
         <v>1790.84</v>
       </c>
-      <c r="E13" s="96">
+      <c r="E13" s="85">
         <v>1206.77</v>
       </c>
-      <c r="F13" s="79">
+      <c r="F13" s="68">
         <v>1628.13</v>
       </c>
-      <c r="G13" s="114">
+      <c r="G13" s="97">
         <v>8962.11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="93" t="s">
+    <row r="14" spans="1:19" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="86">
         <v>21710.65</v>
       </c>
-      <c r="D14" s="97">
+      <c r="D14" s="86">
         <v>26434.920000000002</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="86">
         <v>20220.620000000003</v>
       </c>
-      <c r="F14" s="115">
+      <c r="F14" s="98">
         <v>35441.409999999996</v>
       </c>
-      <c r="G14" s="116">
+      <c r="G14" s="99">
         <v>103807.6</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="89"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="76"/>
+    <row r="15" spans="1:19" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="78"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="65"/>
     </row>
-    <row r="16" spans="1:17" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="108" t="s">
+    <row r="16" spans="1:19" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="76"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="65"/>
     </row>
-    <row r="17" spans="2:15" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="109"/>
-      <c r="C17" s="99" t="s">
+    <row r="17" spans="2:15" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="115"/>
+      <c r="C17" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="99" t="s">
+      <c r="E17" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="80" t="s">
+      <c r="F17" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="62" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="85" t="s">
+    <row r="18" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="100">
+      <c r="C18" s="89">
         <v>12462.87</v>
       </c>
-      <c r="D18" s="100">
+      <c r="D18" s="89">
         <v>8256.9699999999993</v>
       </c>
-      <c r="E18" s="100">
+      <c r="E18" s="89">
         <v>10884.65</v>
       </c>
-      <c r="F18" s="81">
+      <c r="F18" s="70">
         <v>18995.599999999999</v>
       </c>
-      <c r="G18" s="62">
+      <c r="G18" s="58">
         <v>50600.09</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="86" t="s">
+    <row r="19" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="101">
+      <c r="C19" s="90">
         <v>2533.2399999999998</v>
       </c>
-      <c r="D19" s="101">
+      <c r="D19" s="90">
         <v>5855.47</v>
       </c>
-      <c r="E19" s="101">
+      <c r="E19" s="90">
         <v>8525.14</v>
       </c>
-      <c r="F19" s="82">
+      <c r="F19" s="71">
         <v>11253.21</v>
       </c>
-      <c r="G19" s="63">
+      <c r="G19" s="59">
         <v>28167.059999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="87" t="s">
+    <row r="20" spans="2:15" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="102">
+      <c r="C20" s="91">
         <v>8755.24</v>
       </c>
-      <c r="D20" s="102">
+      <c r="D20" s="91">
         <v>7562.22</v>
       </c>
-      <c r="E20" s="102">
+      <c r="E20" s="91">
         <v>5221.5600000000004</v>
       </c>
-      <c r="F20" s="83">
+      <c r="F20" s="72">
         <v>3256.47</v>
       </c>
-      <c r="G20" s="64">
+      <c r="G20" s="60">
         <v>24795.49</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="88" t="s">
+    <row r="21" spans="2:15" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="103">
+      <c r="C21" s="92">
         <v>23751.35</v>
       </c>
-      <c r="D21" s="103">
+      <c r="D21" s="92">
         <v>21674.66</v>
       </c>
-      <c r="E21" s="103">
+      <c r="E21" s="92">
         <v>24631.350000000002</v>
       </c>
-      <c r="F21" s="117">
+      <c r="F21" s="100">
         <v>33505.279999999999</v>
       </c>
-      <c r="G21" s="118">
+      <c r="G21" s="101">
         <v>103562.64</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="89"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="76"/>
+    <row r="22" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="78"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="65"/>
     </row>
     <row r="23" spans="2:15" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="76"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="65"/>
     </row>
-    <row r="24" spans="2:15" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="107"/>
-      <c r="C24" s="104" t="s">
+    <row r="24" spans="2:15" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="117"/>
+      <c r="C24" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="104" t="s">
+      <c r="E24" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="121" t="s">
+      <c r="G24" s="104" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="84" t="s">
+    <row r="25" spans="2:15" ht="10.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="105">
+      <c r="C25" s="94">
         <v>-2040.6999999999971</v>
       </c>
-      <c r="D25" s="105">
+      <c r="D25" s="94">
         <v>4760.260000000002</v>
       </c>
-      <c r="E25" s="105">
+      <c r="E25" s="94">
         <v>-4410.7299999999996</v>
       </c>
-      <c r="F25" s="119">
+      <c r="F25" s="102">
         <v>1936.1299999999974</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="103">
         <v>244.96</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:15" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:15" ht="10.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:XFD4"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:S2"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7598,87 +7664,87 @@
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="48" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" style="48" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="48" customWidth="1"/>
+    <col min="1" max="1" width="1.54296875" style="48" customWidth="1"/>
+    <col min="2" max="2" width="2.81640625" style="48" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" style="48" customWidth="1"/>
     <col min="4" max="4" width="100" style="48" customWidth="1"/>
-    <col min="5" max="5" width="1.5703125" style="48" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="48"/>
+    <col min="5" max="5" width="1.54296875" style="48" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="B2" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
     </row>
-    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="74" t="s">
+    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="121" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="74"/>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="121"/>
       <c r="D5" s="51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="74"/>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="121"/>
       <c r="D6" s="52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="74"/>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="121"/>
       <c r="D7" s="51" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="74"/>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="121"/>
       <c r="D8" s="53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="49"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="74" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="121" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="50" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="74"/>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="121"/>
       <c r="D11" s="51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="74"/>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="121"/>
       <c r="D12" s="52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="74"/>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="121"/>
       <c r="D13" s="54" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection password="C7C0" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">

</xml_diff>